<commit_message>
Landscape New Extraction Fixes
</commit_message>
<xml_diff>
--- a/Nicolas Sparkling Dataset.xlsx
+++ b/Nicolas Sparkling Dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaellaASHRAF\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaellaASHRAF\OneDrive - Pricing One SA\Documents\Slide-Automate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B6B3EF-643D-431F-8266-A37F733EDE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F80FD6A-9C75-416D-971B-343F5801EEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -689,7 +689,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Raphaella ASHRAF" refreshedDate="45895.938107870374" backgroundQuery="1" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Raphaella ASHRAF" refreshedDate="45896.53486550926" backgroundQuery="1" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="0"/>
   <cacheHierarchies count="2647">

</xml_diff>